<commit_message>
new asci values formatted and switched for brts
</commit_message>
<xml_diff>
--- a/input_data/Gage_sample_site_queries.xlsx
+++ b/input_data/Gage_sample_site_queries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katieirving/Documents/git/asci_ffm_2019/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BABA0356-ECDD-2843-AA2D-4A4F26384C54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB87F50-94DF-FB4A-B306-2E2FE239FEED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5720" yWindow="1100" windowWidth="28040" windowHeight="17440" xr2:uid="{01621698-0B39-D84A-B510-3F66A917510F}"/>
   </bookViews>
@@ -644,7 +644,7 @@
   <dimension ref="A1:D59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -669,7 +669,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
@@ -683,7 +683,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>72</v>
       </c>
@@ -697,7 +697,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -711,7 +711,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -725,7 +725,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
@@ -739,7 +739,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>32</v>
       </c>
@@ -753,7 +753,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
@@ -767,7 +767,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>34</v>
       </c>
@@ -781,7 +781,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>35</v>
       </c>
@@ -795,7 +795,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>36</v>
       </c>
@@ -837,7 +837,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>39</v>
       </c>
@@ -851,7 +851,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>40</v>
       </c>
@@ -901,7 +901,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>42</v>
       </c>
@@ -915,7 +915,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>43</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>48</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>50</v>
       </c>
@@ -1093,7 +1093,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>51</v>
       </c>
@@ -1118,7 +1118,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>52</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>53</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>54</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>55</v>
       </c>

</xml_diff>